<commit_message>
Hoàn thiện các chức năng và cơ sở dữ liệu
</commit_message>
<xml_diff>
--- a/CSDL/Matkhau-Tai khoan.xlsx
+++ b/CSDL/Matkhau-Tai khoan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiet\Documents\NHOM 9\Trương Tuấn Kiệt_49.01.103.043\Nhóm No 4991_Quản lý quán Cà phê\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiet\Documents\NHOM 9\Trương Tuấn Kiệt_49.01.103.043\Nhóm No 4991_Quản lý quán Cà phê\JazzCoffe\CSDL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F005B32-585E-44A1-9CBD-5916EE997B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60719E0-9256-4B20-A4AF-5115518FFE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="8170" xr2:uid="{A45A876E-36CF-4D47-B6A1-BC45AAF2B53A}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -470,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1204</v>
+        <v>120420</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>

</xml_diff>